<commit_message>
Se cambie el analisis de la entrevista
</commit_message>
<xml_diff>
--- a/doc/trim1/1_gestion_proyecto/2_levantamiento_informacion/1_recoleccion_informacion.xlsx
+++ b/doc/trim1/1_gestion_proyecto/2_levantamiento_informacion/1_recoleccion_informacion.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C498912-4A15-467E-A25A-C954B0DEDA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C5F0D1-CBC9-4F75-85AE-CF0CAB8200F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="712" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="129">
   <si>
     <t>&lt;Nombre Proyecto&gt;</t>
   </si>
@@ -519,7 +519,16 @@
     <t>Exhibición</t>
   </si>
   <si>
-    <t>ANÁLISIS DE RECOLECCIÓN DE DATOS.
+    <t>0003</t>
+  </si>
+  <si>
+    <t>Se cambia el analisis de la entevista</t>
+  </si>
+  <si>
+    <t>10/03/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ANÁLISIS DE RECOLECCIÓN DE DATOS.
 Con el objetivo de obtener información acerca de la empresa XXX ubicada en XXX la cual se dedica a la comercialización de productos varios, se plantearon diferentes métodos de recolección de datos los cuales irán siendo nombrados posteriormente.
 Para un sondeo previo acerca de la empresa anteriormente mencionada se utiliza el método de cuestionario vía electrónica, con ayuda de la herramienta Google forms, con el fin de obtener resultados óptimos se plantean objetivos para la investigación los cuales son:
 •	Conocer los procesos de la empresa.
@@ -528,7 +537,7 @@
 •	Identificar oportunidades de mejora en los procesos para desarrollar un software.
 •	Conocer procesos manuales que se puedan automatizar.
 Definiendo los objetivos del cuestionario se procede a realizar preguntas de tipo cerrado, las cuales tienen como objetivo que las mismas se enfoquen en respuestas concretas, y no da mucha importancia a las experiencias o sentimientos del propietario de la empresa; esto puesto que ello se realiza para dar una idea general de la empresa y los procesos que la misma tiene, como se puede observar en la siguiente imagen un ejemplo de las interrogantes.
-                                                                                                                                                                                                                                                                                                                                                                                 Ilustración 1.Preguntas cuestionario conocimiento general Google forms.
+Ilustración 1.Preguntas cuestionario conocimiento general Google forms.
 Fuente: Google forms
 Las preguntas realizadas en su totalidad con sus respectivas respuestas se podrán consultar en el Anexo A
 Como resultado del cuestionario se tuvieron en cuenta respuestas clave para obtener información que pueda alimentar los objetivos propuesto, identificando los siguientes procesos con los que cuenta la empresa:
@@ -557,6 +566,8 @@
 El dueño de la empresa menciona que el producto de control de ventas es algo que el definitivamente tiene que hacer, y lo genera a diario, este proceso lo realiza en un cuaderno, donde coloca la fecha, el valor del producto, la cantidad y de que producto se trata.
 Cuando un cliente requiere una factura el dueño utiliza un cuadro con unos productos, y este le pone la X al producto que se compró, posteriormente en la noche el mismo envía un correo para realizar así la factura electrónica.
 Cuando un producto se vence el dueño comenta la novedad a los proveedores y ellos realizan el cambio.
+Para realizar un pedido a los proveedores se realiza de 2 maneras, las cuales pueden ser directamente en la pagina web del proveedor, donde este escoge envía dinero y espera el producto; La otra manera es con el agente de campo designado por el proveedor, donde se escogen los productos y se paga y al día siguiente llegan estos, aproximadamente demorando entre 1 a dos días.
+El control monetario de la empresa es realizado por un contador contratado independiente, este requiere las ventas diarias de la empresa.
 La conclusión que obtengas de tu investigación marcará el rumbo de la toma de decisiones de la empresa, así que presenta tu reporte de manera clara, enumera los pasos que seguiste para la obtención de esos resultados. 
 Tras terminar con la entrevista se le solicita al dueño permiso para observar la tienda, y tomar fotos de los productos generados por los procesos, esto con el método de observación, tomando apuntes en la libreta de campo.
 Algunas de las fotografías obtenidas fueron:
@@ -565,7 +576,8 @@
 Ilustración 3. Exhibición
 Fuente propia
 Ilustración 4. Documentos acopiados
-Fuente propia</t>
+Fuente propia
+</t>
   </si>
 </sst>
 </file>
@@ -1626,7 +1638,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1781,24 +1793,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="47" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -1817,18 +1821,26 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="37" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1856,7 +1868,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="49" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1893,6 +1904,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="49" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1986,6 +1998,9 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4157,15 +4172,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>88447</xdr:colOff>
+      <xdr:colOff>126547</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>204105</xdr:rowOff>
+      <xdr:rowOff>108855</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1149803</xdr:colOff>
+      <xdr:colOff>1187903</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>476250</xdr:rowOff>
+      <xdr:rowOff>381000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4187,8 +4202,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="88447" y="5728605"/>
-          <a:ext cx="3871231" cy="1939020"/>
+          <a:off x="126547" y="5766705"/>
+          <a:ext cx="3880756" cy="2005695"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4531,8 +4546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:IV87"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView showGridLines="0" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -4557,55 +4572,55 @@
       <c r="F2" s="2"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
     </row>
     <row r="7" spans="1:11" ht="30">
-      <c r="C7" s="93" t="s">
+      <c r="C7" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="94"/>
-      <c r="E7" s="95"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="89"/>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:11" ht="30">
-      <c r="C8" s="93" t="s">
+      <c r="C8" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="94"/>
-      <c r="E8" s="95"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="89"/>
     </row>
     <row r="10" spans="1:11" s="43" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="97"/>
-      <c r="B10" s="97"/>
-      <c r="C10" s="97"/>
-      <c r="D10" s="97"/>
-      <c r="E10" s="97"/>
-      <c r="F10" s="97"/>
-      <c r="G10" s="97"/>
-      <c r="H10" s="97"/>
-      <c r="I10" s="97"/>
-      <c r="J10" s="97"/>
-      <c r="K10" s="97"/>
+      <c r="A10" s="91"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="91"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
     </row>
     <row r="11" spans="1:11" ht="15" thickTop="1"/>
     <row r="13" spans="1:11" ht="30">
-      <c r="B13" s="96" t="s">
+      <c r="B13" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="96"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="96"/>
-      <c r="F13" s="96"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
     </row>
     <row r="15" spans="1:11" ht="15" thickBot="1">
       <c r="B15" s="2"/>
@@ -4616,56 +4631,56 @@
       <c r="B16" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="98" t="s">
+      <c r="C16" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="D16" s="98"/>
-      <c r="E16" s="98"/>
-      <c r="F16" s="98"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="82"/>
+      <c r="F16" s="82"/>
     </row>
     <row r="17" spans="1:16" ht="18">
       <c r="B17" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="99" t="s">
+      <c r="C17" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="99"/>
-      <c r="E17" s="99"/>
-      <c r="F17" s="99"/>
+      <c r="D17" s="83"/>
+      <c r="E17" s="83"/>
+      <c r="F17" s="83"/>
     </row>
     <row r="18" spans="1:16" ht="18">
       <c r="B18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="99" t="s">
+      <c r="C18" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="99"/>
-      <c r="E18" s="99"/>
-      <c r="F18" s="99"/>
+      <c r="D18" s="83"/>
+      <c r="E18" s="83"/>
+      <c r="F18" s="83"/>
     </row>
     <row r="19" spans="1:16" ht="19.899999999999999" customHeight="1" thickBot="1">
       <c r="A19" s="29"/>
       <c r="B19" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="100" t="s">
+      <c r="C19" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="100"/>
-      <c r="E19" s="100"/>
-      <c r="F19" s="100"/>
+      <c r="D19" s="84"/>
+      <c r="E19" s="84"/>
+      <c r="F19" s="84"/>
     </row>
     <row r="20" spans="1:16" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A20" s="29"/>
       <c r="B20" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="101" t="s">
+      <c r="C20" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="101"/>
+      <c r="D20" s="85"/>
       <c r="E20" s="7" t="s">
         <v>10</v>
       </c>
@@ -4675,13 +4690,13 @@
     </row>
     <row r="21" spans="1:16" ht="19.899999999999999" customHeight="1">
       <c r="A21" s="29"/>
-      <c r="B21" s="90" t="s">
+      <c r="B21" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="83" t="s">
+      <c r="C21" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="83"/>
+      <c r="D21" s="100"/>
       <c r="E21" s="9" t="s">
         <v>13</v>
       </c>
@@ -4691,9 +4706,9 @@
     </row>
     <row r="22" spans="1:16" ht="36.75" thickBot="1">
       <c r="A22" s="29"/>
-      <c r="B22" s="91"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="84"/>
+      <c r="B22" s="99"/>
+      <c r="C22" s="93"/>
+      <c r="D22" s="93"/>
       <c r="E22" s="10" t="s">
         <v>14</v>
       </c>
@@ -4723,10 +4738,10 @@
       <c r="C26" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="86" t="s">
+      <c r="D26" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="86"/>
+      <c r="E26" s="94"/>
       <c r="F26" s="16" t="s">
         <v>20</v>
       </c>
@@ -4738,10 +4753,10 @@
       <c r="C27" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="87" t="s">
+      <c r="D27" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="87"/>
+      <c r="E27" s="95"/>
       <c r="F27" s="19" t="s">
         <v>50</v>
       </c>
@@ -4753,61 +4768,69 @@
       <c r="C28" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="87" t="s">
+      <c r="D28" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="87"/>
+      <c r="E28" s="95"/>
       <c r="F28" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="25.5" customHeight="1">
-      <c r="B29" s="20"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="88"/>
-      <c r="E29" s="88"/>
-      <c r="F29" s="8"/>
+    <row r="29" spans="1:16" ht="27.75" customHeight="1">
+      <c r="B29" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="D29" s="156" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="156"/>
+      <c r="F29" s="8" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="30" spans="1:16" ht="25.5" customHeight="1">
       <c r="B30" s="20"/>
       <c r="C30" s="21"/>
-      <c r="D30" s="88"/>
-      <c r="E30" s="88"/>
+      <c r="D30" s="96"/>
+      <c r="E30" s="96"/>
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:16" ht="25.5" customHeight="1">
       <c r="B31" s="20"/>
       <c r="C31" s="21"/>
-      <c r="D31" s="88"/>
-      <c r="E31" s="88"/>
+      <c r="D31" s="96"/>
+      <c r="E31" s="96"/>
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:16" ht="25.5" customHeight="1">
       <c r="B32" s="20"/>
       <c r="C32" s="21"/>
-      <c r="D32" s="88"/>
-      <c r="E32" s="88"/>
+      <c r="D32" s="96"/>
+      <c r="E32" s="96"/>
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:13" ht="25.5" customHeight="1">
       <c r="B33" s="20"/>
       <c r="C33" s="21"/>
-      <c r="D33" s="88"/>
-      <c r="E33" s="88"/>
+      <c r="D33" s="96"/>
+      <c r="E33" s="96"/>
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:13" ht="25.5" customHeight="1">
       <c r="B34" s="20"/>
       <c r="C34" s="21"/>
-      <c r="D34" s="88"/>
-      <c r="E34" s="88"/>
+      <c r="D34" s="96"/>
+      <c r="E34" s="96"/>
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:13" ht="25.5" customHeight="1" thickBot="1">
       <c r="B35" s="22"/>
       <c r="C35" s="23"/>
-      <c r="D35" s="89"/>
-      <c r="E35" s="89"/>
+      <c r="D35" s="97"/>
+      <c r="E35" s="97"/>
       <c r="F35" s="11"/>
     </row>
     <row r="36" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1">
@@ -4821,52 +4844,52 @@
     </row>
     <row r="38" spans="1:13" ht="30" customHeight="1" thickBot="1"/>
     <row r="39" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B39" s="85" t="s">
+      <c r="B39" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="85"/>
-      <c r="D39" s="85"/>
-      <c r="E39" s="85"/>
-      <c r="F39" s="85"/>
+      <c r="C39" s="92"/>
+      <c r="D39" s="92"/>
+      <c r="E39" s="92"/>
+      <c r="F39" s="92"/>
     </row>
     <row r="40" spans="1:13" ht="25.5" customHeight="1" thickTop="1">
-      <c r="B40" s="82"/>
-      <c r="C40" s="82"/>
-      <c r="D40" s="82"/>
-      <c r="E40" s="82"/>
-      <c r="F40" s="82"/>
+      <c r="B40" s="101"/>
+      <c r="C40" s="101"/>
+      <c r="D40" s="101"/>
+      <c r="E40" s="101"/>
+      <c r="F40" s="101"/>
     </row>
     <row r="41" spans="1:13" ht="25.5" customHeight="1">
-      <c r="B41" s="83"/>
-      <c r="C41" s="83"/>
-      <c r="D41" s="83"/>
-      <c r="E41" s="83"/>
-      <c r="F41" s="83"/>
+      <c r="B41" s="100"/>
+      <c r="C41" s="100"/>
+      <c r="D41" s="100"/>
+      <c r="E41" s="100"/>
+      <c r="F41" s="100"/>
       <c r="J41" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="25.5" customHeight="1">
-      <c r="B42" s="83"/>
-      <c r="C42" s="83"/>
-      <c r="D42" s="83"/>
-      <c r="E42" s="83"/>
-      <c r="F42" s="83"/>
+      <c r="B42" s="100"/>
+      <c r="C42" s="100"/>
+      <c r="D42" s="100"/>
+      <c r="E42" s="100"/>
+      <c r="F42" s="100"/>
     </row>
     <row r="43" spans="1:13" ht="25.5" customHeight="1">
-      <c r="B43" s="83"/>
-      <c r="C43" s="83"/>
-      <c r="D43" s="83"/>
-      <c r="E43" s="83"/>
-      <c r="F43" s="83"/>
+      <c r="B43" s="100"/>
+      <c r="C43" s="100"/>
+      <c r="D43" s="100"/>
+      <c r="E43" s="100"/>
+      <c r="F43" s="100"/>
       <c r="G43" s="24"/>
     </row>
     <row r="44" spans="1:13" ht="25.5" customHeight="1" thickBot="1">
-      <c r="B44" s="84"/>
-      <c r="C44" s="84"/>
-      <c r="D44" s="84"/>
-      <c r="E44" s="84"/>
-      <c r="F44" s="84"/>
+      <c r="B44" s="93"/>
+      <c r="C44" s="93"/>
+      <c r="D44" s="93"/>
+      <c r="E44" s="93"/>
+      <c r="F44" s="93"/>
     </row>
     <row r="45" spans="1:13" ht="19.899999999999999" customHeight="1" thickTop="1">
       <c r="A45" s="25"/>
@@ -5182,18 +5205,11 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
     <mergeCell ref="B39:F39"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="D26:E26"/>
@@ -5208,11 +5224,18 @@
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C20:D20"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="3.937007874015748E-2" bottom="3.937007874015748E-2" header="0" footer="0"/>
@@ -5287,16 +5310,16 @@
       <c r="J5" s="107"/>
     </row>
     <row r="6" spans="1:253" s="43" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A6" s="97"/>
-      <c r="B6" s="97"/>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="97"/>
-      <c r="H6" s="97"/>
-      <c r="I6" s="97"/>
-      <c r="J6" s="97"/>
+      <c r="A6" s="91"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
     </row>
     <row r="7" spans="1:253" ht="15" thickTop="1"/>
     <row r="8" spans="1:253" ht="15" thickBot="1">
@@ -5630,52 +5653,52 @@
     <row r="5" spans="1:12">
       <c r="A5" s="55"/>
       <c r="B5" s="56"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
-      <c r="H5" s="111"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="123"/>
       <c r="I5" s="56"/>
       <c r="J5" s="56"/>
       <c r="K5" s="57"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="58"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
       <c r="K6" s="59"/>
     </row>
     <row r="7" spans="1:12" ht="30">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="94"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="123"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="88"/>
+      <c r="J7" s="88"/>
+      <c r="K7" s="122"/>
     </row>
     <row r="8" spans="1:12" ht="30">
-      <c r="A8" s="122" t="s">
+      <c r="A8" s="121" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="123"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="122"/>
     </row>
     <row r="9" spans="1:12" ht="15" thickBot="1">
       <c r="A9" s="60"/>
@@ -5691,742 +5714,742 @@
       <c r="K9" s="62"/>
     </row>
     <row r="10" spans="1:12" s="43" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="121"/>
-      <c r="B10" s="121"/>
-      <c r="C10" s="121"/>
-      <c r="D10" s="121"/>
-      <c r="E10" s="121"/>
-      <c r="F10" s="121"/>
-      <c r="G10" s="121"/>
-      <c r="H10" s="121"/>
-      <c r="I10" s="121"/>
-      <c r="J10" s="121"/>
-      <c r="K10" s="121"/>
+      <c r="A10" s="120"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="120"/>
+      <c r="D10" s="120"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="120"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="120"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="112" t="s">
+      <c r="A11" s="111" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="113"/>
-      <c r="C11" s="113"/>
-      <c r="D11" s="113"/>
-      <c r="E11" s="113"/>
-      <c r="F11" s="113"/>
-      <c r="G11" s="113"/>
-      <c r="H11" s="113"/>
-      <c r="I11" s="113"/>
-      <c r="J11" s="113"/>
-      <c r="K11" s="114"/>
+      <c r="B11" s="112"/>
+      <c r="C11" s="112"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="112"/>
+      <c r="F11" s="112"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="112"/>
+      <c r="I11" s="112"/>
+      <c r="J11" s="112"/>
+      <c r="K11" s="113"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="115"/>
-      <c r="B12" s="116"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
-      <c r="G12" s="116"/>
-      <c r="H12" s="116"/>
-      <c r="I12" s="116"/>
-      <c r="J12" s="116"/>
-      <c r="K12" s="117"/>
+      <c r="A12" s="114"/>
+      <c r="B12" s="115"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="115"/>
+      <c r="F12" s="115"/>
+      <c r="G12" s="115"/>
+      <c r="H12" s="115"/>
+      <c r="I12" s="115"/>
+      <c r="J12" s="115"/>
+      <c r="K12" s="116"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="115"/>
-      <c r="B13" s="116"/>
-      <c r="C13" s="116"/>
-      <c r="D13" s="116"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="116"/>
-      <c r="G13" s="116"/>
-      <c r="H13" s="116"/>
-      <c r="I13" s="116"/>
-      <c r="J13" s="116"/>
-      <c r="K13" s="117"/>
+      <c r="A13" s="114"/>
+      <c r="B13" s="115"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="115"/>
+      <c r="I13" s="115"/>
+      <c r="J13" s="115"/>
+      <c r="K13" s="116"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="115"/>
-      <c r="B14" s="116"/>
-      <c r="C14" s="116"/>
-      <c r="D14" s="116"/>
-      <c r="E14" s="116"/>
-      <c r="F14" s="116"/>
-      <c r="G14" s="116"/>
-      <c r="H14" s="116"/>
-      <c r="I14" s="116"/>
-      <c r="J14" s="116"/>
-      <c r="K14" s="117"/>
+      <c r="A14" s="114"/>
+      <c r="B14" s="115"/>
+      <c r="C14" s="115"/>
+      <c r="D14" s="115"/>
+      <c r="E14" s="115"/>
+      <c r="F14" s="115"/>
+      <c r="G14" s="115"/>
+      <c r="H14" s="115"/>
+      <c r="I14" s="115"/>
+      <c r="J14" s="115"/>
+      <c r="K14" s="116"/>
     </row>
     <row r="15" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A15" s="115"/>
-      <c r="B15" s="116"/>
-      <c r="C15" s="116"/>
-      <c r="D15" s="116"/>
-      <c r="E15" s="116"/>
-      <c r="F15" s="116"/>
-      <c r="G15" s="116"/>
-      <c r="H15" s="116"/>
-      <c r="I15" s="116"/>
-      <c r="J15" s="116"/>
-      <c r="K15" s="117"/>
+      <c r="A15" s="114"/>
+      <c r="B15" s="115"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="115"/>
+      <c r="E15" s="115"/>
+      <c r="F15" s="115"/>
+      <c r="G15" s="115"/>
+      <c r="H15" s="115"/>
+      <c r="I15" s="115"/>
+      <c r="J15" s="115"/>
+      <c r="K15" s="116"/>
       <c r="L15" s="34"/>
     </row>
     <row r="16" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A16" s="115"/>
-      <c r="B16" s="116"/>
-      <c r="C16" s="116"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="116"/>
-      <c r="F16" s="116"/>
-      <c r="G16" s="116"/>
-      <c r="H16" s="116"/>
-      <c r="I16" s="116"/>
-      <c r="J16" s="116"/>
-      <c r="K16" s="117"/>
+      <c r="A16" s="114"/>
+      <c r="B16" s="115"/>
+      <c r="C16" s="115"/>
+      <c r="D16" s="115"/>
+      <c r="E16" s="115"/>
+      <c r="F16" s="115"/>
+      <c r="G16" s="115"/>
+      <c r="H16" s="115"/>
+      <c r="I16" s="115"/>
+      <c r="J16" s="115"/>
+      <c r="K16" s="116"/>
       <c r="L16" s="34"/>
     </row>
     <row r="17" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A17" s="115"/>
-      <c r="B17" s="116"/>
-      <c r="C17" s="116"/>
-      <c r="D17" s="116"/>
-      <c r="E17" s="116"/>
-      <c r="F17" s="116"/>
-      <c r="G17" s="116"/>
-      <c r="H17" s="116"/>
-      <c r="I17" s="116"/>
-      <c r="J17" s="116"/>
-      <c r="K17" s="117"/>
+      <c r="A17" s="114"/>
+      <c r="B17" s="115"/>
+      <c r="C17" s="115"/>
+      <c r="D17" s="115"/>
+      <c r="E17" s="115"/>
+      <c r="F17" s="115"/>
+      <c r="G17" s="115"/>
+      <c r="H17" s="115"/>
+      <c r="I17" s="115"/>
+      <c r="J17" s="115"/>
+      <c r="K17" s="116"/>
       <c r="L17" s="34"/>
     </row>
     <row r="18" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A18" s="115"/>
-      <c r="B18" s="116"/>
-      <c r="C18" s="116"/>
-      <c r="D18" s="116"/>
-      <c r="E18" s="116"/>
-      <c r="F18" s="116"/>
-      <c r="G18" s="116"/>
-      <c r="H18" s="116"/>
-      <c r="I18" s="116"/>
-      <c r="J18" s="116"/>
-      <c r="K18" s="117"/>
+      <c r="A18" s="114"/>
+      <c r="B18" s="115"/>
+      <c r="C18" s="115"/>
+      <c r="D18" s="115"/>
+      <c r="E18" s="115"/>
+      <c r="F18" s="115"/>
+      <c r="G18" s="115"/>
+      <c r="H18" s="115"/>
+      <c r="I18" s="115"/>
+      <c r="J18" s="115"/>
+      <c r="K18" s="116"/>
       <c r="L18" s="34"/>
     </row>
     <row r="19" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A19" s="115"/>
-      <c r="B19" s="116"/>
-      <c r="C19" s="116"/>
-      <c r="D19" s="116"/>
-      <c r="E19" s="116"/>
-      <c r="F19" s="116"/>
-      <c r="G19" s="116"/>
-      <c r="H19" s="116"/>
-      <c r="I19" s="116"/>
-      <c r="J19" s="116"/>
-      <c r="K19" s="117"/>
+      <c r="A19" s="114"/>
+      <c r="B19" s="115"/>
+      <c r="C19" s="115"/>
+      <c r="D19" s="115"/>
+      <c r="E19" s="115"/>
+      <c r="F19" s="115"/>
+      <c r="G19" s="115"/>
+      <c r="H19" s="115"/>
+      <c r="I19" s="115"/>
+      <c r="J19" s="115"/>
+      <c r="K19" s="116"/>
       <c r="L19" s="34"/>
     </row>
     <row r="20" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A20" s="115"/>
-      <c r="B20" s="116"/>
-      <c r="C20" s="116"/>
-      <c r="D20" s="116"/>
-      <c r="E20" s="116"/>
-      <c r="F20" s="116"/>
-      <c r="G20" s="116"/>
-      <c r="H20" s="116"/>
-      <c r="I20" s="116"/>
-      <c r="J20" s="116"/>
-      <c r="K20" s="117"/>
+      <c r="A20" s="114"/>
+      <c r="B20" s="115"/>
+      <c r="C20" s="115"/>
+      <c r="D20" s="115"/>
+      <c r="E20" s="115"/>
+      <c r="F20" s="115"/>
+      <c r="G20" s="115"/>
+      <c r="H20" s="115"/>
+      <c r="I20" s="115"/>
+      <c r="J20" s="115"/>
+      <c r="K20" s="116"/>
       <c r="L20" s="34"/>
     </row>
     <row r="21" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A21" s="115"/>
-      <c r="B21" s="116"/>
-      <c r="C21" s="116"/>
-      <c r="D21" s="116"/>
-      <c r="E21" s="116"/>
-      <c r="F21" s="116"/>
-      <c r="G21" s="116"/>
-      <c r="H21" s="116"/>
-      <c r="I21" s="116"/>
-      <c r="J21" s="116"/>
-      <c r="K21" s="117"/>
+      <c r="A21" s="114"/>
+      <c r="B21" s="115"/>
+      <c r="C21" s="115"/>
+      <c r="D21" s="115"/>
+      <c r="E21" s="115"/>
+      <c r="F21" s="115"/>
+      <c r="G21" s="115"/>
+      <c r="H21" s="115"/>
+      <c r="I21" s="115"/>
+      <c r="J21" s="115"/>
+      <c r="K21" s="116"/>
       <c r="L21" s="34"/>
     </row>
     <row r="22" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A22" s="115"/>
-      <c r="B22" s="116"/>
-      <c r="C22" s="116"/>
-      <c r="D22" s="116"/>
-      <c r="E22" s="116"/>
-      <c r="F22" s="116"/>
-      <c r="G22" s="116"/>
-      <c r="H22" s="116"/>
-      <c r="I22" s="116"/>
-      <c r="J22" s="116"/>
-      <c r="K22" s="117"/>
+      <c r="A22" s="114"/>
+      <c r="B22" s="115"/>
+      <c r="C22" s="115"/>
+      <c r="D22" s="115"/>
+      <c r="E22" s="115"/>
+      <c r="F22" s="115"/>
+      <c r="G22" s="115"/>
+      <c r="H22" s="115"/>
+      <c r="I22" s="115"/>
+      <c r="J22" s="115"/>
+      <c r="K22" s="116"/>
       <c r="L22" s="34"/>
     </row>
     <row r="23" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A23" s="115"/>
-      <c r="B23" s="116"/>
-      <c r="C23" s="116"/>
-      <c r="D23" s="116"/>
-      <c r="E23" s="116"/>
-      <c r="F23" s="116"/>
-      <c r="G23" s="116"/>
-      <c r="H23" s="116"/>
-      <c r="I23" s="116"/>
-      <c r="J23" s="116"/>
-      <c r="K23" s="117"/>
+      <c r="A23" s="114"/>
+      <c r="B23" s="115"/>
+      <c r="C23" s="115"/>
+      <c r="D23" s="115"/>
+      <c r="E23" s="115"/>
+      <c r="F23" s="115"/>
+      <c r="G23" s="115"/>
+      <c r="H23" s="115"/>
+      <c r="I23" s="115"/>
+      <c r="J23" s="115"/>
+      <c r="K23" s="116"/>
       <c r="L23" s="34"/>
     </row>
     <row r="24" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A24" s="115"/>
-      <c r="B24" s="116"/>
-      <c r="C24" s="116"/>
-      <c r="D24" s="116"/>
-      <c r="E24" s="116"/>
-      <c r="F24" s="116"/>
-      <c r="G24" s="116"/>
-      <c r="H24" s="116"/>
-      <c r="I24" s="116"/>
-      <c r="J24" s="116"/>
-      <c r="K24" s="117"/>
+      <c r="A24" s="114"/>
+      <c r="B24" s="115"/>
+      <c r="C24" s="115"/>
+      <c r="D24" s="115"/>
+      <c r="E24" s="115"/>
+      <c r="F24" s="115"/>
+      <c r="G24" s="115"/>
+      <c r="H24" s="115"/>
+      <c r="I24" s="115"/>
+      <c r="J24" s="115"/>
+      <c r="K24" s="116"/>
       <c r="L24" s="34"/>
     </row>
     <row r="25" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A25" s="115"/>
-      <c r="B25" s="116"/>
-      <c r="C25" s="116"/>
-      <c r="D25" s="116"/>
-      <c r="E25" s="116"/>
-      <c r="F25" s="116"/>
-      <c r="G25" s="116"/>
-      <c r="H25" s="116"/>
-      <c r="I25" s="116"/>
-      <c r="J25" s="116"/>
-      <c r="K25" s="117"/>
+      <c r="A25" s="114"/>
+      <c r="B25" s="115"/>
+      <c r="C25" s="115"/>
+      <c r="D25" s="115"/>
+      <c r="E25" s="115"/>
+      <c r="F25" s="115"/>
+      <c r="G25" s="115"/>
+      <c r="H25" s="115"/>
+      <c r="I25" s="115"/>
+      <c r="J25" s="115"/>
+      <c r="K25" s="116"/>
       <c r="L25" s="34"/>
     </row>
     <row r="26" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A26" s="115"/>
-      <c r="B26" s="116"/>
-      <c r="C26" s="116"/>
-      <c r="D26" s="116"/>
-      <c r="E26" s="116"/>
-      <c r="F26" s="116"/>
-      <c r="G26" s="116"/>
-      <c r="H26" s="116"/>
-      <c r="I26" s="116"/>
-      <c r="J26" s="116"/>
-      <c r="K26" s="117"/>
+      <c r="A26" s="114"/>
+      <c r="B26" s="115"/>
+      <c r="C26" s="115"/>
+      <c r="D26" s="115"/>
+      <c r="E26" s="115"/>
+      <c r="F26" s="115"/>
+      <c r="G26" s="115"/>
+      <c r="H26" s="115"/>
+      <c r="I26" s="115"/>
+      <c r="J26" s="115"/>
+      <c r="K26" s="116"/>
       <c r="L26" s="34"/>
     </row>
     <row r="27" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A27" s="115"/>
-      <c r="B27" s="116"/>
-      <c r="C27" s="116"/>
-      <c r="D27" s="116"/>
-      <c r="E27" s="116"/>
-      <c r="F27" s="116"/>
-      <c r="G27" s="116"/>
-      <c r="H27" s="116"/>
-      <c r="I27" s="116"/>
-      <c r="J27" s="116"/>
-      <c r="K27" s="117"/>
+      <c r="A27" s="114"/>
+      <c r="B27" s="115"/>
+      <c r="C27" s="115"/>
+      <c r="D27" s="115"/>
+      <c r="E27" s="115"/>
+      <c r="F27" s="115"/>
+      <c r="G27" s="115"/>
+      <c r="H27" s="115"/>
+      <c r="I27" s="115"/>
+      <c r="J27" s="115"/>
+      <c r="K27" s="116"/>
       <c r="L27" s="34"/>
     </row>
     <row r="28" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A28" s="115"/>
-      <c r="B28" s="116"/>
-      <c r="C28" s="116"/>
-      <c r="D28" s="116"/>
-      <c r="E28" s="116"/>
-      <c r="F28" s="116"/>
-      <c r="G28" s="116"/>
-      <c r="H28" s="116"/>
-      <c r="I28" s="116"/>
-      <c r="J28" s="116"/>
-      <c r="K28" s="117"/>
+      <c r="A28" s="114"/>
+      <c r="B28" s="115"/>
+      <c r="C28" s="115"/>
+      <c r="D28" s="115"/>
+      <c r="E28" s="115"/>
+      <c r="F28" s="115"/>
+      <c r="G28" s="115"/>
+      <c r="H28" s="115"/>
+      <c r="I28" s="115"/>
+      <c r="J28" s="115"/>
+      <c r="K28" s="116"/>
       <c r="L28" s="34"/>
     </row>
     <row r="29" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A29" s="115"/>
-      <c r="B29" s="116"/>
-      <c r="C29" s="116"/>
-      <c r="D29" s="116"/>
-      <c r="E29" s="116"/>
-      <c r="F29" s="116"/>
-      <c r="G29" s="116"/>
-      <c r="H29" s="116"/>
-      <c r="I29" s="116"/>
-      <c r="J29" s="116"/>
-      <c r="K29" s="117"/>
+      <c r="A29" s="114"/>
+      <c r="B29" s="115"/>
+      <c r="C29" s="115"/>
+      <c r="D29" s="115"/>
+      <c r="E29" s="115"/>
+      <c r="F29" s="115"/>
+      <c r="G29" s="115"/>
+      <c r="H29" s="115"/>
+      <c r="I29" s="115"/>
+      <c r="J29" s="115"/>
+      <c r="K29" s="116"/>
       <c r="L29" s="34"/>
     </row>
     <row r="30" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1">
-      <c r="A30" s="115"/>
-      <c r="B30" s="116"/>
-      <c r="C30" s="116"/>
-      <c r="D30" s="116"/>
-      <c r="E30" s="116"/>
-      <c r="F30" s="116"/>
-      <c r="G30" s="116"/>
-      <c r="H30" s="116"/>
-      <c r="I30" s="116"/>
-      <c r="J30" s="116"/>
-      <c r="K30" s="117"/>
+      <c r="A30" s="114"/>
+      <c r="B30" s="115"/>
+      <c r="C30" s="115"/>
+      <c r="D30" s="115"/>
+      <c r="E30" s="115"/>
+      <c r="F30" s="115"/>
+      <c r="G30" s="115"/>
+      <c r="H30" s="115"/>
+      <c r="I30" s="115"/>
+      <c r="J30" s="115"/>
+      <c r="K30" s="116"/>
       <c r="L30" s="34"/>
     </row>
     <row r="31" spans="1:12" s="1" customFormat="1" ht="19.899999999999999" customHeight="1" thickBot="1">
-      <c r="A31" s="118"/>
-      <c r="B31" s="119"/>
-      <c r="C31" s="119"/>
-      <c r="D31" s="119"/>
-      <c r="E31" s="119"/>
-      <c r="F31" s="119"/>
-      <c r="G31" s="119"/>
-      <c r="H31" s="119"/>
-      <c r="I31" s="119"/>
-      <c r="J31" s="119"/>
-      <c r="K31" s="120"/>
+      <c r="A31" s="117"/>
+      <c r="B31" s="118"/>
+      <c r="C31" s="118"/>
+      <c r="D31" s="118"/>
+      <c r="E31" s="118"/>
+      <c r="F31" s="118"/>
+      <c r="G31" s="118"/>
+      <c r="H31" s="118"/>
+      <c r="I31" s="118"/>
+      <c r="J31" s="118"/>
+      <c r="K31" s="119"/>
       <c r="L31" s="34"/>
     </row>
     <row r="32" spans="1:12" s="1" customFormat="1">
-      <c r="A32" s="112" t="s">
+      <c r="A32" s="111" t="s">
         <v>66</v>
       </c>
-      <c r="B32" s="113"/>
-      <c r="C32" s="113"/>
-      <c r="D32" s="113"/>
-      <c r="E32" s="113"/>
-      <c r="F32" s="113"/>
-      <c r="G32" s="113"/>
-      <c r="H32" s="113"/>
-      <c r="I32" s="113"/>
-      <c r="J32" s="113"/>
-      <c r="K32" s="114"/>
+      <c r="B32" s="112"/>
+      <c r="C32" s="112"/>
+      <c r="D32" s="112"/>
+      <c r="E32" s="112"/>
+      <c r="F32" s="112"/>
+      <c r="G32" s="112"/>
+      <c r="H32" s="112"/>
+      <c r="I32" s="112"/>
+      <c r="J32" s="112"/>
+      <c r="K32" s="113"/>
     </row>
     <row r="33" spans="1:11" s="1" customFormat="1">
-      <c r="A33" s="115"/>
-      <c r="B33" s="116"/>
-      <c r="C33" s="116"/>
-      <c r="D33" s="116"/>
-      <c r="E33" s="116"/>
-      <c r="F33" s="116"/>
-      <c r="G33" s="116"/>
-      <c r="H33" s="116"/>
-      <c r="I33" s="116"/>
-      <c r="J33" s="116"/>
-      <c r="K33" s="117"/>
+      <c r="A33" s="114"/>
+      <c r="B33" s="115"/>
+      <c r="C33" s="115"/>
+      <c r="D33" s="115"/>
+      <c r="E33" s="115"/>
+      <c r="F33" s="115"/>
+      <c r="G33" s="115"/>
+      <c r="H33" s="115"/>
+      <c r="I33" s="115"/>
+      <c r="J33" s="115"/>
+      <c r="K33" s="116"/>
     </row>
     <row r="34" spans="1:11" s="1" customFormat="1">
-      <c r="A34" s="115"/>
-      <c r="B34" s="116"/>
-      <c r="C34" s="116"/>
-      <c r="D34" s="116"/>
-      <c r="E34" s="116"/>
-      <c r="F34" s="116"/>
-      <c r="G34" s="116"/>
-      <c r="H34" s="116"/>
-      <c r="I34" s="116"/>
-      <c r="J34" s="116"/>
-      <c r="K34" s="117"/>
+      <c r="A34" s="114"/>
+      <c r="B34" s="115"/>
+      <c r="C34" s="115"/>
+      <c r="D34" s="115"/>
+      <c r="E34" s="115"/>
+      <c r="F34" s="115"/>
+      <c r="G34" s="115"/>
+      <c r="H34" s="115"/>
+      <c r="I34" s="115"/>
+      <c r="J34" s="115"/>
+      <c r="K34" s="116"/>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="115"/>
-      <c r="B35" s="116"/>
-      <c r="C35" s="116"/>
-      <c r="D35" s="116"/>
-      <c r="E35" s="116"/>
-      <c r="F35" s="116"/>
-      <c r="G35" s="116"/>
-      <c r="H35" s="116"/>
-      <c r="I35" s="116"/>
-      <c r="J35" s="116"/>
-      <c r="K35" s="117"/>
+      <c r="A35" s="114"/>
+      <c r="B35" s="115"/>
+      <c r="C35" s="115"/>
+      <c r="D35" s="115"/>
+      <c r="E35" s="115"/>
+      <c r="F35" s="115"/>
+      <c r="G35" s="115"/>
+      <c r="H35" s="115"/>
+      <c r="I35" s="115"/>
+      <c r="J35" s="115"/>
+      <c r="K35" s="116"/>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="115"/>
-      <c r="B36" s="116"/>
-      <c r="C36" s="116"/>
-      <c r="D36" s="116"/>
-      <c r="E36" s="116"/>
-      <c r="F36" s="116"/>
-      <c r="G36" s="116"/>
-      <c r="H36" s="116"/>
-      <c r="I36" s="116"/>
-      <c r="J36" s="116"/>
-      <c r="K36" s="117"/>
+      <c r="A36" s="114"/>
+      <c r="B36" s="115"/>
+      <c r="C36" s="115"/>
+      <c r="D36" s="115"/>
+      <c r="E36" s="115"/>
+      <c r="F36" s="115"/>
+      <c r="G36" s="115"/>
+      <c r="H36" s="115"/>
+      <c r="I36" s="115"/>
+      <c r="J36" s="115"/>
+      <c r="K36" s="116"/>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="115"/>
-      <c r="B37" s="116"/>
-      <c r="C37" s="116"/>
-      <c r="D37" s="116"/>
-      <c r="E37" s="116"/>
-      <c r="F37" s="116"/>
-      <c r="G37" s="116"/>
-      <c r="H37" s="116"/>
-      <c r="I37" s="116"/>
-      <c r="J37" s="116"/>
-      <c r="K37" s="117"/>
+      <c r="A37" s="114"/>
+      <c r="B37" s="115"/>
+      <c r="C37" s="115"/>
+      <c r="D37" s="115"/>
+      <c r="E37" s="115"/>
+      <c r="F37" s="115"/>
+      <c r="G37" s="115"/>
+      <c r="H37" s="115"/>
+      <c r="I37" s="115"/>
+      <c r="J37" s="115"/>
+      <c r="K37" s="116"/>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="115"/>
-      <c r="B38" s="116"/>
-      <c r="C38" s="116"/>
-      <c r="D38" s="116"/>
-      <c r="E38" s="116"/>
-      <c r="F38" s="116"/>
-      <c r="G38" s="116"/>
-      <c r="H38" s="116"/>
-      <c r="I38" s="116"/>
-      <c r="J38" s="116"/>
-      <c r="K38" s="117"/>
+      <c r="A38" s="114"/>
+      <c r="B38" s="115"/>
+      <c r="C38" s="115"/>
+      <c r="D38" s="115"/>
+      <c r="E38" s="115"/>
+      <c r="F38" s="115"/>
+      <c r="G38" s="115"/>
+      <c r="H38" s="115"/>
+      <c r="I38" s="115"/>
+      <c r="J38" s="115"/>
+      <c r="K38" s="116"/>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="115"/>
-      <c r="B39" s="116"/>
-      <c r="C39" s="116"/>
-      <c r="D39" s="116"/>
-      <c r="E39" s="116"/>
-      <c r="F39" s="116"/>
-      <c r="G39" s="116"/>
-      <c r="H39" s="116"/>
-      <c r="I39" s="116"/>
-      <c r="J39" s="116"/>
-      <c r="K39" s="117"/>
+      <c r="A39" s="114"/>
+      <c r="B39" s="115"/>
+      <c r="C39" s="115"/>
+      <c r="D39" s="115"/>
+      <c r="E39" s="115"/>
+      <c r="F39" s="115"/>
+      <c r="G39" s="115"/>
+      <c r="H39" s="115"/>
+      <c r="I39" s="115"/>
+      <c r="J39" s="115"/>
+      <c r="K39" s="116"/>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="115"/>
-      <c r="B40" s="116"/>
-      <c r="C40" s="116"/>
-      <c r="D40" s="116"/>
-      <c r="E40" s="116"/>
-      <c r="F40" s="116"/>
-      <c r="G40" s="116"/>
-      <c r="H40" s="116"/>
-      <c r="I40" s="116"/>
-      <c r="J40" s="116"/>
-      <c r="K40" s="117"/>
+      <c r="A40" s="114"/>
+      <c r="B40" s="115"/>
+      <c r="C40" s="115"/>
+      <c r="D40" s="115"/>
+      <c r="E40" s="115"/>
+      <c r="F40" s="115"/>
+      <c r="G40" s="115"/>
+      <c r="H40" s="115"/>
+      <c r="I40" s="115"/>
+      <c r="J40" s="115"/>
+      <c r="K40" s="116"/>
     </row>
     <row r="41" spans="1:11">
-      <c r="A41" s="115"/>
-      <c r="B41" s="116"/>
-      <c r="C41" s="116"/>
-      <c r="D41" s="116"/>
-      <c r="E41" s="116"/>
-      <c r="F41" s="116"/>
-      <c r="G41" s="116"/>
-      <c r="H41" s="116"/>
-      <c r="I41" s="116"/>
-      <c r="J41" s="116"/>
-      <c r="K41" s="117"/>
+      <c r="A41" s="114"/>
+      <c r="B41" s="115"/>
+      <c r="C41" s="115"/>
+      <c r="D41" s="115"/>
+      <c r="E41" s="115"/>
+      <c r="F41" s="115"/>
+      <c r="G41" s="115"/>
+      <c r="H41" s="115"/>
+      <c r="I41" s="115"/>
+      <c r="J41" s="115"/>
+      <c r="K41" s="116"/>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="115"/>
-      <c r="B42" s="116"/>
-      <c r="C42" s="116"/>
-      <c r="D42" s="116"/>
-      <c r="E42" s="116"/>
-      <c r="F42" s="116"/>
-      <c r="G42" s="116"/>
-      <c r="H42" s="116"/>
-      <c r="I42" s="116"/>
-      <c r="J42" s="116"/>
-      <c r="K42" s="117"/>
+      <c r="A42" s="114"/>
+      <c r="B42" s="115"/>
+      <c r="C42" s="115"/>
+      <c r="D42" s="115"/>
+      <c r="E42" s="115"/>
+      <c r="F42" s="115"/>
+      <c r="G42" s="115"/>
+      <c r="H42" s="115"/>
+      <c r="I42" s="115"/>
+      <c r="J42" s="115"/>
+      <c r="K42" s="116"/>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="115"/>
-      <c r="B43" s="116"/>
-      <c r="C43" s="116"/>
-      <c r="D43" s="116"/>
-      <c r="E43" s="116"/>
-      <c r="F43" s="116"/>
-      <c r="G43" s="116"/>
-      <c r="H43" s="116"/>
-      <c r="I43" s="116"/>
-      <c r="J43" s="116"/>
-      <c r="K43" s="117"/>
+      <c r="A43" s="114"/>
+      <c r="B43" s="115"/>
+      <c r="C43" s="115"/>
+      <c r="D43" s="115"/>
+      <c r="E43" s="115"/>
+      <c r="F43" s="115"/>
+      <c r="G43" s="115"/>
+      <c r="H43" s="115"/>
+      <c r="I43" s="115"/>
+      <c r="J43" s="115"/>
+      <c r="K43" s="116"/>
     </row>
     <row r="44" spans="1:11">
-      <c r="A44" s="115"/>
-      <c r="B44" s="116"/>
-      <c r="C44" s="116"/>
-      <c r="D44" s="116"/>
-      <c r="E44" s="116"/>
-      <c r="F44" s="116"/>
-      <c r="G44" s="116"/>
-      <c r="H44" s="116"/>
-      <c r="I44" s="116"/>
-      <c r="J44" s="116"/>
-      <c r="K44" s="117"/>
+      <c r="A44" s="114"/>
+      <c r="B44" s="115"/>
+      <c r="C44" s="115"/>
+      <c r="D44" s="115"/>
+      <c r="E44" s="115"/>
+      <c r="F44" s="115"/>
+      <c r="G44" s="115"/>
+      <c r="H44" s="115"/>
+      <c r="I44" s="115"/>
+      <c r="J44" s="115"/>
+      <c r="K44" s="116"/>
     </row>
     <row r="45" spans="1:11" ht="15" thickBot="1">
-      <c r="A45" s="118"/>
-      <c r="B45" s="119"/>
-      <c r="C45" s="119"/>
-      <c r="D45" s="119"/>
-      <c r="E45" s="119"/>
-      <c r="F45" s="119"/>
-      <c r="G45" s="119"/>
-      <c r="H45" s="119"/>
-      <c r="I45" s="119"/>
-      <c r="J45" s="119"/>
-      <c r="K45" s="120"/>
+      <c r="A45" s="117"/>
+      <c r="B45" s="118"/>
+      <c r="C45" s="118"/>
+      <c r="D45" s="118"/>
+      <c r="E45" s="118"/>
+      <c r="F45" s="118"/>
+      <c r="G45" s="118"/>
+      <c r="H45" s="118"/>
+      <c r="I45" s="118"/>
+      <c r="J45" s="118"/>
+      <c r="K45" s="119"/>
     </row>
     <row r="46" spans="1:11">
-      <c r="A46" s="112" t="s">
+      <c r="A46" s="111" t="s">
         <v>68</v>
       </c>
-      <c r="B46" s="113"/>
-      <c r="C46" s="113"/>
-      <c r="D46" s="113"/>
-      <c r="E46" s="113"/>
-      <c r="F46" s="113"/>
-      <c r="G46" s="113"/>
-      <c r="H46" s="113"/>
-      <c r="I46" s="113"/>
-      <c r="J46" s="113"/>
-      <c r="K46" s="114"/>
+      <c r="B46" s="112"/>
+      <c r="C46" s="112"/>
+      <c r="D46" s="112"/>
+      <c r="E46" s="112"/>
+      <c r="F46" s="112"/>
+      <c r="G46" s="112"/>
+      <c r="H46" s="112"/>
+      <c r="I46" s="112"/>
+      <c r="J46" s="112"/>
+      <c r="K46" s="113"/>
     </row>
     <row r="47" spans="1:11">
-      <c r="A47" s="115"/>
-      <c r="B47" s="116"/>
-      <c r="C47" s="116"/>
-      <c r="D47" s="116"/>
-      <c r="E47" s="116"/>
-      <c r="F47" s="116"/>
-      <c r="G47" s="116"/>
-      <c r="H47" s="116"/>
-      <c r="I47" s="116"/>
-      <c r="J47" s="116"/>
-      <c r="K47" s="117"/>
+      <c r="A47" s="114"/>
+      <c r="B47" s="115"/>
+      <c r="C47" s="115"/>
+      <c r="D47" s="115"/>
+      <c r="E47" s="115"/>
+      <c r="F47" s="115"/>
+      <c r="G47" s="115"/>
+      <c r="H47" s="115"/>
+      <c r="I47" s="115"/>
+      <c r="J47" s="115"/>
+      <c r="K47" s="116"/>
     </row>
     <row r="48" spans="1:11">
-      <c r="A48" s="115"/>
-      <c r="B48" s="116"/>
-      <c r="C48" s="116"/>
-      <c r="D48" s="116"/>
-      <c r="E48" s="116"/>
-      <c r="F48" s="116"/>
-      <c r="G48" s="116"/>
-      <c r="H48" s="116"/>
-      <c r="I48" s="116"/>
-      <c r="J48" s="116"/>
-      <c r="K48" s="117"/>
+      <c r="A48" s="114"/>
+      <c r="B48" s="115"/>
+      <c r="C48" s="115"/>
+      <c r="D48" s="115"/>
+      <c r="E48" s="115"/>
+      <c r="F48" s="115"/>
+      <c r="G48" s="115"/>
+      <c r="H48" s="115"/>
+      <c r="I48" s="115"/>
+      <c r="J48" s="115"/>
+      <c r="K48" s="116"/>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="115"/>
-      <c r="B49" s="116"/>
-      <c r="C49" s="116"/>
-      <c r="D49" s="116"/>
-      <c r="E49" s="116"/>
-      <c r="F49" s="116"/>
-      <c r="G49" s="116"/>
-      <c r="H49" s="116"/>
-      <c r="I49" s="116"/>
-      <c r="J49" s="116"/>
-      <c r="K49" s="117"/>
+      <c r="A49" s="114"/>
+      <c r="B49" s="115"/>
+      <c r="C49" s="115"/>
+      <c r="D49" s="115"/>
+      <c r="E49" s="115"/>
+      <c r="F49" s="115"/>
+      <c r="G49" s="115"/>
+      <c r="H49" s="115"/>
+      <c r="I49" s="115"/>
+      <c r="J49" s="115"/>
+      <c r="K49" s="116"/>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="115"/>
-      <c r="B50" s="116"/>
-      <c r="C50" s="116"/>
-      <c r="D50" s="116"/>
-      <c r="E50" s="116"/>
-      <c r="F50" s="116"/>
-      <c r="G50" s="116"/>
-      <c r="H50" s="116"/>
-      <c r="I50" s="116"/>
-      <c r="J50" s="116"/>
-      <c r="K50" s="117"/>
+      <c r="A50" s="114"/>
+      <c r="B50" s="115"/>
+      <c r="C50" s="115"/>
+      <c r="D50" s="115"/>
+      <c r="E50" s="115"/>
+      <c r="F50" s="115"/>
+      <c r="G50" s="115"/>
+      <c r="H50" s="115"/>
+      <c r="I50" s="115"/>
+      <c r="J50" s="115"/>
+      <c r="K50" s="116"/>
     </row>
     <row r="51" spans="1:11">
-      <c r="A51" s="115"/>
-      <c r="B51" s="116"/>
-      <c r="C51" s="116"/>
-      <c r="D51" s="116"/>
-      <c r="E51" s="116"/>
-      <c r="F51" s="116"/>
-      <c r="G51" s="116"/>
-      <c r="H51" s="116"/>
-      <c r="I51" s="116"/>
-      <c r="J51" s="116"/>
-      <c r="K51" s="117"/>
+      <c r="A51" s="114"/>
+      <c r="B51" s="115"/>
+      <c r="C51" s="115"/>
+      <c r="D51" s="115"/>
+      <c r="E51" s="115"/>
+      <c r="F51" s="115"/>
+      <c r="G51" s="115"/>
+      <c r="H51" s="115"/>
+      <c r="I51" s="115"/>
+      <c r="J51" s="115"/>
+      <c r="K51" s="116"/>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="115"/>
-      <c r="B52" s="116"/>
-      <c r="C52" s="116"/>
-      <c r="D52" s="116"/>
-      <c r="E52" s="116"/>
-      <c r="F52" s="116"/>
-      <c r="G52" s="116"/>
-      <c r="H52" s="116"/>
-      <c r="I52" s="116"/>
-      <c r="J52" s="116"/>
-      <c r="K52" s="117"/>
+      <c r="A52" s="114"/>
+      <c r="B52" s="115"/>
+      <c r="C52" s="115"/>
+      <c r="D52" s="115"/>
+      <c r="E52" s="115"/>
+      <c r="F52" s="115"/>
+      <c r="G52" s="115"/>
+      <c r="H52" s="115"/>
+      <c r="I52" s="115"/>
+      <c r="J52" s="115"/>
+      <c r="K52" s="116"/>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="115"/>
-      <c r="B53" s="116"/>
-      <c r="C53" s="116"/>
-      <c r="D53" s="116"/>
-      <c r="E53" s="116"/>
-      <c r="F53" s="116"/>
-      <c r="G53" s="116"/>
-      <c r="H53" s="116"/>
-      <c r="I53" s="116"/>
-      <c r="J53" s="116"/>
-      <c r="K53" s="117"/>
+      <c r="A53" s="114"/>
+      <c r="B53" s="115"/>
+      <c r="C53" s="115"/>
+      <c r="D53" s="115"/>
+      <c r="E53" s="115"/>
+      <c r="F53" s="115"/>
+      <c r="G53" s="115"/>
+      <c r="H53" s="115"/>
+      <c r="I53" s="115"/>
+      <c r="J53" s="115"/>
+      <c r="K53" s="116"/>
     </row>
     <row r="54" spans="1:11">
-      <c r="A54" s="115"/>
-      <c r="B54" s="116"/>
-      <c r="C54" s="116"/>
-      <c r="D54" s="116"/>
-      <c r="E54" s="116"/>
-      <c r="F54" s="116"/>
-      <c r="G54" s="116"/>
-      <c r="H54" s="116"/>
-      <c r="I54" s="116"/>
-      <c r="J54" s="116"/>
-      <c r="K54" s="117"/>
+      <c r="A54" s="114"/>
+      <c r="B54" s="115"/>
+      <c r="C54" s="115"/>
+      <c r="D54" s="115"/>
+      <c r="E54" s="115"/>
+      <c r="F54" s="115"/>
+      <c r="G54" s="115"/>
+      <c r="H54" s="115"/>
+      <c r="I54" s="115"/>
+      <c r="J54" s="115"/>
+      <c r="K54" s="116"/>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="115"/>
-      <c r="B55" s="116"/>
-      <c r="C55" s="116"/>
-      <c r="D55" s="116"/>
-      <c r="E55" s="116"/>
-      <c r="F55" s="116"/>
-      <c r="G55" s="116"/>
-      <c r="H55" s="116"/>
-      <c r="I55" s="116"/>
-      <c r="J55" s="116"/>
-      <c r="K55" s="117"/>
+      <c r="A55" s="114"/>
+      <c r="B55" s="115"/>
+      <c r="C55" s="115"/>
+      <c r="D55" s="115"/>
+      <c r="E55" s="115"/>
+      <c r="F55" s="115"/>
+      <c r="G55" s="115"/>
+      <c r="H55" s="115"/>
+      <c r="I55" s="115"/>
+      <c r="J55" s="115"/>
+      <c r="K55" s="116"/>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56" s="115"/>
-      <c r="B56" s="116"/>
-      <c r="C56" s="116"/>
-      <c r="D56" s="116"/>
-      <c r="E56" s="116"/>
-      <c r="F56" s="116"/>
-      <c r="G56" s="116"/>
-      <c r="H56" s="116"/>
-      <c r="I56" s="116"/>
-      <c r="J56" s="116"/>
-      <c r="K56" s="117"/>
+      <c r="A56" s="114"/>
+      <c r="B56" s="115"/>
+      <c r="C56" s="115"/>
+      <c r="D56" s="115"/>
+      <c r="E56" s="115"/>
+      <c r="F56" s="115"/>
+      <c r="G56" s="115"/>
+      <c r="H56" s="115"/>
+      <c r="I56" s="115"/>
+      <c r="J56" s="115"/>
+      <c r="K56" s="116"/>
     </row>
     <row r="57" spans="1:11">
-      <c r="A57" s="115"/>
-      <c r="B57" s="116"/>
-      <c r="C57" s="116"/>
-      <c r="D57" s="116"/>
-      <c r="E57" s="116"/>
-      <c r="F57" s="116"/>
-      <c r="G57" s="116"/>
-      <c r="H57" s="116"/>
-      <c r="I57" s="116"/>
-      <c r="J57" s="116"/>
-      <c r="K57" s="117"/>
+      <c r="A57" s="114"/>
+      <c r="B57" s="115"/>
+      <c r="C57" s="115"/>
+      <c r="D57" s="115"/>
+      <c r="E57" s="115"/>
+      <c r="F57" s="115"/>
+      <c r="G57" s="115"/>
+      <c r="H57" s="115"/>
+      <c r="I57" s="115"/>
+      <c r="J57" s="115"/>
+      <c r="K57" s="116"/>
     </row>
     <row r="58" spans="1:11">
-      <c r="A58" s="115"/>
-      <c r="B58" s="116"/>
-      <c r="C58" s="116"/>
-      <c r="D58" s="116"/>
-      <c r="E58" s="116"/>
-      <c r="F58" s="116"/>
-      <c r="G58" s="116"/>
-      <c r="H58" s="116"/>
-      <c r="I58" s="116"/>
-      <c r="J58" s="116"/>
-      <c r="K58" s="117"/>
+      <c r="A58" s="114"/>
+      <c r="B58" s="115"/>
+      <c r="C58" s="115"/>
+      <c r="D58" s="115"/>
+      <c r="E58" s="115"/>
+      <c r="F58" s="115"/>
+      <c r="G58" s="115"/>
+      <c r="H58" s="115"/>
+      <c r="I58" s="115"/>
+      <c r="J58" s="115"/>
+      <c r="K58" s="116"/>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="115"/>
-      <c r="B59" s="116"/>
-      <c r="C59" s="116"/>
-      <c r="D59" s="116"/>
-      <c r="E59" s="116"/>
-      <c r="F59" s="116"/>
-      <c r="G59" s="116"/>
-      <c r="H59" s="116"/>
-      <c r="I59" s="116"/>
-      <c r="J59" s="116"/>
-      <c r="K59" s="117"/>
+      <c r="A59" s="114"/>
+      <c r="B59" s="115"/>
+      <c r="C59" s="115"/>
+      <c r="D59" s="115"/>
+      <c r="E59" s="115"/>
+      <c r="F59" s="115"/>
+      <c r="G59" s="115"/>
+      <c r="H59" s="115"/>
+      <c r="I59" s="115"/>
+      <c r="J59" s="115"/>
+      <c r="K59" s="116"/>
     </row>
     <row r="60" spans="1:11">
-      <c r="A60" s="115"/>
-      <c r="B60" s="116"/>
-      <c r="C60" s="116"/>
-      <c r="D60" s="116"/>
-      <c r="E60" s="116"/>
-      <c r="F60" s="116"/>
-      <c r="G60" s="116"/>
-      <c r="H60" s="116"/>
-      <c r="I60" s="116"/>
-      <c r="J60" s="116"/>
-      <c r="K60" s="117"/>
+      <c r="A60" s="114"/>
+      <c r="B60" s="115"/>
+      <c r="C60" s="115"/>
+      <c r="D60" s="115"/>
+      <c r="E60" s="115"/>
+      <c r="F60" s="115"/>
+      <c r="G60" s="115"/>
+      <c r="H60" s="115"/>
+      <c r="I60" s="115"/>
+      <c r="J60" s="115"/>
+      <c r="K60" s="116"/>
     </row>
     <row r="61" spans="1:11">
-      <c r="A61" s="115"/>
-      <c r="B61" s="116"/>
-      <c r="C61" s="116"/>
-      <c r="D61" s="116"/>
-      <c r="E61" s="116"/>
-      <c r="F61" s="116"/>
-      <c r="G61" s="116"/>
-      <c r="H61" s="116"/>
-      <c r="I61" s="116"/>
-      <c r="J61" s="116"/>
-      <c r="K61" s="117"/>
+      <c r="A61" s="114"/>
+      <c r="B61" s="115"/>
+      <c r="C61" s="115"/>
+      <c r="D61" s="115"/>
+      <c r="E61" s="115"/>
+      <c r="F61" s="115"/>
+      <c r="G61" s="115"/>
+      <c r="H61" s="115"/>
+      <c r="I61" s="115"/>
+      <c r="J61" s="115"/>
+      <c r="K61" s="116"/>
     </row>
     <row r="62" spans="1:11">
-      <c r="A62" s="115"/>
-      <c r="B62" s="116"/>
-      <c r="C62" s="116"/>
-      <c r="D62" s="116"/>
-      <c r="E62" s="116"/>
-      <c r="F62" s="116"/>
-      <c r="G62" s="116"/>
-      <c r="H62" s="116"/>
-      <c r="I62" s="116"/>
-      <c r="J62" s="116"/>
-      <c r="K62" s="117"/>
+      <c r="A62" s="114"/>
+      <c r="B62" s="115"/>
+      <c r="C62" s="115"/>
+      <c r="D62" s="115"/>
+      <c r="E62" s="115"/>
+      <c r="F62" s="115"/>
+      <c r="G62" s="115"/>
+      <c r="H62" s="115"/>
+      <c r="I62" s="115"/>
+      <c r="J62" s="115"/>
+      <c r="K62" s="116"/>
     </row>
     <row r="63" spans="1:11">
-      <c r="A63" s="115"/>
-      <c r="B63" s="116"/>
-      <c r="C63" s="116"/>
-      <c r="D63" s="116"/>
-      <c r="E63" s="116"/>
-      <c r="F63" s="116"/>
-      <c r="G63" s="116"/>
-      <c r="H63" s="116"/>
-      <c r="I63" s="116"/>
-      <c r="J63" s="116"/>
-      <c r="K63" s="117"/>
+      <c r="A63" s="114"/>
+      <c r="B63" s="115"/>
+      <c r="C63" s="115"/>
+      <c r="D63" s="115"/>
+      <c r="E63" s="115"/>
+      <c r="F63" s="115"/>
+      <c r="G63" s="115"/>
+      <c r="H63" s="115"/>
+      <c r="I63" s="115"/>
+      <c r="J63" s="115"/>
+      <c r="K63" s="116"/>
     </row>
     <row r="64" spans="1:11" ht="15" thickBot="1">
-      <c r="A64" s="118"/>
-      <c r="B64" s="119"/>
-      <c r="C64" s="119"/>
-      <c r="D64" s="119"/>
-      <c r="E64" s="119"/>
-      <c r="F64" s="119"/>
-      <c r="G64" s="119"/>
-      <c r="H64" s="119"/>
-      <c r="I64" s="119"/>
-      <c r="J64" s="119"/>
-      <c r="K64" s="120"/>
+      <c r="A64" s="117"/>
+      <c r="B64" s="118"/>
+      <c r="C64" s="118"/>
+      <c r="D64" s="118"/>
+      <c r="E64" s="118"/>
+      <c r="F64" s="118"/>
+      <c r="G64" s="118"/>
+      <c r="H64" s="118"/>
+      <c r="I64" s="118"/>
+      <c r="J64" s="118"/>
+      <c r="K64" s="119"/>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="39"/>
@@ -6505,12 +6528,12 @@
     <row r="5" spans="1:257">
       <c r="A5" s="55"/>
       <c r="B5" s="56"/>
-      <c r="C5" s="111"/>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="111"/>
-      <c r="H5" s="111"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="123"/>
       <c r="I5" s="56"/>
       <c r="J5" s="56"/>
       <c r="K5" s="57"/>
@@ -6518,42 +6541,42 @@
     </row>
     <row r="6" spans="1:257">
       <c r="A6" s="58"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
       <c r="K6" s="59"/>
       <c r="L6" s="34"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="94"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="123"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="88"/>
+      <c r="J7" s="88"/>
+      <c r="K7" s="122"/>
       <c r="L7" s="34"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="A8" s="122" t="s">
+      <c r="A8" s="121" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="123"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="122"/>
       <c r="L8" s="34"/>
     </row>
     <row r="9" spans="1:257" ht="15" thickBot="1">
@@ -6571,17 +6594,17 @@
       <c r="L9" s="34"/>
     </row>
     <row r="10" spans="1:257" s="43" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="121"/>
-      <c r="B10" s="121"/>
-      <c r="C10" s="121"/>
-      <c r="D10" s="121"/>
-      <c r="E10" s="121"/>
-      <c r="F10" s="121"/>
-      <c r="G10" s="121"/>
-      <c r="H10" s="121"/>
-      <c r="I10" s="121"/>
-      <c r="J10" s="121"/>
-      <c r="K10" s="121"/>
+      <c r="A10" s="120"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="120"/>
+      <c r="D10" s="120"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="120"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="120"/>
+      <c r="I10" s="120"/>
+      <c r="J10" s="120"/>
+      <c r="K10" s="120"/>
     </row>
     <row r="11" spans="1:257" ht="15.75" customHeight="1">
       <c r="A11" s="124" t="s">
@@ -7312,16 +7335,16 @@
     </row>
     <row r="10" spans="1:257" s="43" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
       <c r="A10" s="142"/>
-      <c r="B10" s="97"/>
-      <c r="C10" s="97"/>
-      <c r="D10" s="97"/>
-      <c r="E10" s="97"/>
-      <c r="F10" s="97"/>
-      <c r="G10" s="97"/>
-      <c r="H10" s="97"/>
-      <c r="I10" s="97"/>
-      <c r="J10" s="97"/>
-      <c r="K10" s="97"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="91"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
       <c r="L10" s="77"/>
     </row>
     <row r="11" spans="1:257" ht="15" thickTop="1"/>
@@ -7489,54 +7512,54 @@
     </row>
     <row r="5" spans="1:257">
       <c r="A5" s="58"/>
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
       <c r="L5" s="59"/>
       <c r="M5" s="34"/>
     </row>
     <row r="6" spans="1:257">
       <c r="A6" s="58"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
       <c r="L6" s="59"/>
       <c r="M6" s="34"/>
     </row>
     <row r="7" spans="1:257" ht="30">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="94"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="95"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="88"/>
+      <c r="J7" s="88"/>
+      <c r="K7" s="89"/>
       <c r="L7" s="59"/>
       <c r="M7" s="34"/>
     </row>
     <row r="8" spans="1:257" ht="30">
-      <c r="A8" s="122" t="s">
+      <c r="A8" s="121" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="95"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="89"/>
       <c r="L8" s="59"/>
       <c r="M8" s="34"/>
     </row>
@@ -7930,7 +7953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:IV226"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A47" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:K226"/>
     </sheetView>
   </sheetViews>
@@ -7973,56 +7996,56 @@
       <c r="IV4" s="1"/>
     </row>
     <row r="5" spans="1:256">
-      <c r="C5" s="92"/>
-      <c r="D5" s="92"/>
-      <c r="E5" s="92"/>
-      <c r="F5" s="92"/>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
       <c r="IT5" s="1"/>
       <c r="IU5" s="1"/>
       <c r="IV5" s="1"/>
     </row>
     <row r="6" spans="1:256">
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
       <c r="IT6" s="1"/>
       <c r="IU6" s="1"/>
       <c r="IV6" s="1"/>
     </row>
     <row r="7" spans="1:256" ht="30">
-      <c r="A7" s="93" t="s">
+      <c r="A7" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="94"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="95"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="88"/>
+      <c r="J7" s="88"/>
+      <c r="K7" s="89"/>
       <c r="IT7" s="1"/>
       <c r="IU7" s="1"/>
       <c r="IV7" s="1"/>
     </row>
     <row r="8" spans="1:256" ht="30">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="95"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="88"/>
+      <c r="E8" s="88"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="88"/>
+      <c r="H8" s="88"/>
+      <c r="I8" s="88"/>
+      <c r="J8" s="88"/>
+      <c r="K8" s="89"/>
       <c r="IT8" s="1"/>
       <c r="IU8" s="1"/>
       <c r="IV8" s="1"/>
@@ -8033,17 +8056,17 @@
       <c r="IV9" s="1"/>
     </row>
     <row r="10" spans="1:256" s="43" customFormat="1" ht="5.0999999999999996" customHeight="1" thickBot="1">
-      <c r="A10" s="97"/>
-      <c r="B10" s="97"/>
-      <c r="C10" s="97"/>
-      <c r="D10" s="97"/>
-      <c r="E10" s="97"/>
-      <c r="F10" s="97"/>
-      <c r="G10" s="97"/>
-      <c r="H10" s="97"/>
-      <c r="I10" s="97"/>
-      <c r="J10" s="97"/>
-      <c r="K10" s="97"/>
+      <c r="A10" s="91"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="91"/>
+      <c r="E10" s="91"/>
+      <c r="F10" s="91"/>
+      <c r="G10" s="91"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="91"/>
+      <c r="J10" s="91"/>
+      <c r="K10" s="91"/>
     </row>
     <row r="11" spans="1:256" ht="15" thickTop="1">
       <c r="IT11" s="1"/>
@@ -8052,7 +8075,7 @@
     </row>
     <row r="12" spans="1:256" ht="15.75" customHeight="1">
       <c r="A12" s="150" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B12" s="150"/>
       <c r="C12" s="150"/>

</xml_diff>